<commit_message>
Got inheritance down via rocket classes
</commit_message>
<xml_diff>
--- a/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
+++ b/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Luis\Documents\School\Aersp424\FINAL_PROJECT\ReferenceMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD8364B-3538-4171-B97F-95635184B931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA09DCA8-4B84-4C00-9540-05DD62772284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="75" windowWidth="24885" windowHeight="14415" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="2490" yWindow="225" windowWidth="24885" windowHeight="14415" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,6 +394,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -711,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +798,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B6">
@@ -1108,7 +1109,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B27">
@@ -1125,7 +1126,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B28">
@@ -1142,7 +1143,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B29">
@@ -1159,7 +1160,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B30">
@@ -1173,7 +1174,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B31">

</xml_diff>

<commit_message>
Finished with the rocket-related classes
</commit_message>
<xml_diff>
--- a/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
+++ b/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Luis\Documents\School\Aersp424\FINAL_PROJECT\ReferenceMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA09DCA8-4B84-4C00-9540-05DD62772284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1222B4A8-780B-47C4-A954-487BAC3BD7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="225" windowWidth="24885" windowHeight="14415" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="1710" yWindow="2610" windowWidth="24885" windowHeight="14415" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,7 +394,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -712,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +746,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B3">
@@ -764,7 +763,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B4">
@@ -781,7 +780,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B5">
@@ -827,7 +826,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B8">
@@ -909,7 +908,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B13">
@@ -1046,7 +1045,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B23">
@@ -1063,7 +1062,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B24">
@@ -1080,7 +1079,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B25">
@@ -1109,7 +1108,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27">

</xml_diff>

<commit_message>
Working on orbit equations
</commit_message>
<xml_diff>
--- a/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
+++ b/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Luis\Documents\School\Aersp424\FINAL_PROJECT\ReferenceMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209C4494-6A14-4910-AA60-400B5FDA80AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC393093-91FE-40CD-A831-A9C1212731B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1710" yWindow="1185" windowWidth="24885" windowHeight="14415" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="122" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="122" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +922,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B14">
@@ -964,7 +964,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B17">
@@ -1006,7 +1006,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B20">

</xml_diff>

<commit_message>
Working on added premade rockets
</commit_message>
<xml_diff>
--- a/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
+++ b/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Luis\Documents\School\Aersp424\FINAL_PROJECT\ReferenceMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC393093-91FE-40CD-A831-A9C1212731B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FAC4EF-DDD1-4A73-8B04-FBB917ECCD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="1185" windowWidth="24885" windowHeight="14415" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="330" yWindow="1215" windowWidth="24885" windowHeight="14415" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,6 +394,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -711,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="122" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,7 +878,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B11">
@@ -992,7 +993,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B19">
@@ -1034,7 +1035,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B22">
@@ -1187,7 +1188,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B32">

</xml_diff>

<commit_message>
Finished console based rocket builder
</commit_message>
<xml_diff>
--- a/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
+++ b/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Luis\Documents\School\Aersp424\FINAL_PROJECT\ReferenceMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FAC4EF-DDD1-4A73-8B04-FBB917ECCD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A27ACC-02E5-4A01-8385-9E4C11D96D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="1215" windowWidth="24885" windowHeight="14415" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="330" yWindow="1185" windowWidth="24885" windowHeight="14415" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,7 +394,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -713,7 +712,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1034,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" t="s">
         <v>44</v>
       </c>
       <c r="B22">

</xml_diff>

<commit_message>
Highlighted the areas that we need to finish
</commit_message>
<xml_diff>
--- a/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
+++ b/ReferenceMaterial/Project_Grading_Rubric_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Luis\Documents\School\Aersp424\FINAL_PROJECT\ReferenceMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A27ACC-02E5-4A01-8385-9E4C11D96D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1154C91E-FDFA-4AB6-93C1-4EB4797735E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="1185" windowWidth="24885" windowHeight="14415" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="330" yWindow="1185" windowWidth="27915" windowHeight="14415" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -327,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +343,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -375,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -394,6 +400,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -711,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="122" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +850,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B9">
@@ -860,7 +867,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B10">
@@ -891,7 +898,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B12">
@@ -1034,7 +1041,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B22">
@@ -1108,7 +1115,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B27">

</xml_diff>